<commit_message>
Mehr gemacht mit stosse
</commit_message>
<xml_diff>
--- a/Versuch6/datasets/stosse/stosse.xlsx
+++ b/Versuch6/datasets/stosse/stosse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele Calvanese\Uni\Grundpraktikum\Versuch6\datasets\stosse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{55D3CE41-2F5B-4931-8C3A-1E3CEF9B6585}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{37809D01-8DB1-4AC8-9C34-517CC6B594A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22932" windowHeight="5616" activeTab="3" xr2:uid="{31778D45-214A-4E9C-9F87-862031E98347}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="29">
   <si>
     <t>m1</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t>m1+m2</t>
+  </si>
+  <si>
+    <t>v_rel</t>
+  </si>
+  <si>
+    <t>vs_rel</t>
+  </si>
+  <si>
+    <t>vs_rel_err</t>
+  </si>
+  <si>
+    <t>v_rel_err</t>
+  </si>
+  <si>
+    <t>eta</t>
+  </si>
+  <si>
+    <t>eta_err</t>
   </si>
 </sst>
 </file>
@@ -448,15 +466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0B2733-9449-4FE5-9091-A4C75772EFDB}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,25 +527,43 @@
         <v>11</v>
       </c>
       <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AC1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AD1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>206.137</v>
       </c>
@@ -589,31 +625,55 @@
         <v>0.10199730245942783</v>
       </c>
       <c r="S2">
+        <f>G2-M2</f>
+        <v>81.477599999999995</v>
+      </c>
+      <c r="T2">
+        <f>SQRT(H2^2+N2^2)</f>
+        <v>0.14434487106232768</v>
+      </c>
+      <c r="U2">
+        <f>J2-P2</f>
+        <v>-78.68180000000001</v>
+      </c>
+      <c r="V2">
+        <f>SQRT(K2^2+Q2^2)</f>
+        <v>0.14414999177939625</v>
+      </c>
+      <c r="W2">
+        <f>U2^2/S2^2</f>
+        <v>0.93254998077662465</v>
+      </c>
+      <c r="X2">
+        <f>2*ABS(U2/S2)*SQRT((V2/S2)^2+(U2*T2/S2^2)^2)</f>
+        <v>4.7532553099981691E-3</v>
+      </c>
+      <c r="Z2">
         <f>(G2*A2+M2*C2)/(A2+C2)</f>
         <v>0.5862938512864756</v>
       </c>
-      <c r="T2">
+      <c r="AA2">
         <f>SQRT(((G2/E2-(A2*G2+C2*M2)/E2^2)*B2)^2+((M2/E2-(A2*G2+C2*M2)/E2^2)*D2)^2+(A2*H2/E2)^2+(C2*N2/E2)^2)</f>
         <v>7.2172887668996946E-2</v>
       </c>
-      <c r="U2">
+      <c r="AB2">
         <f>(J2*A2+P2*C2)/(A2+C2)</f>
         <v>0.61489294753217272</v>
       </c>
-      <c r="V2">
+      <c r="AC2">
         <f>SQRT(((J2/E2-(A2*J2+C2*P2)/E2^2)*B2)^2+((P2/E2-(A2*J2+C2*P2)/E2^2)*D2)^2+(A2*K2/E2)^2+(C2*Q2/E2)^2)</f>
         <v>7.2075082151281819E-2</v>
       </c>
-      <c r="W2">
-        <f>S2-U2</f>
+      <c r="AD2">
+        <f>Z2-AB2</f>
         <v>-2.859909624569712E-2</v>
       </c>
-      <c r="X2">
-        <f>SQRT(T2^2+V2^2)</f>
+      <c r="AE2">
+        <f>SQRT(AA2^2+AC2^2)</f>
         <v>0.10199874107848426</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2</f>
         <v>206.137</v>
@@ -679,33 +739,57 @@
         <v>0.10237839906933495</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S6" si="10">(G3*A3+M3*C3)/(A3+C3)</f>
+        <f t="shared" ref="S3:S6" si="10">G3-M3</f>
+        <v>91.662300000000002</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T6" si="11">SQRT(H3^2+N3^2)</f>
+        <v>0.1451109998449463</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U6" si="12">J3-P3</f>
+        <v>-87.867999999999995</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V6" si="13">SQRT(K3^2+Q3^2)</f>
+        <v>0.14481541655500632</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W6" si="14">U3^2/S3^2</f>
+        <v>0.91892481998851328</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X6" si="15">2*ABS(U3/S3)*SQRT((V3/S3)^2+(U3*T3/S3^2)^2)</f>
+        <v>4.1999829367139682E-3</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z6" si="16">(G3*A3+M3*C3)/(A3+C3)</f>
         <v>-1.9256673027199895E-3</v>
       </c>
-      <c r="T3">
+      <c r="AA3">
         <f>SQRT(((G3/E3-(A3*G3+C3*M3)/E3^2)*B3)^2+((M3/E3-(A3*G3+C3*M3)/E3^2)*D3)^2+(A3*H3/E3)^2+(C3*N3/E3)^2)</f>
         <v>7.2555802678224673E-2</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U6" si="11">(J3*A3+P3*C3)/(A3+C3)</f>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB6" si="17">(J3*A3+P3*C3)/(A3+C3)</f>
         <v>-0.29357082001483287</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V6" si="12">SQRT(((J3/E3-(A3*J3+C3*P3)/E3^2)*B3)^2+((P3/E3-(A3*J3+C3*P3)/E3^2)*D3)^2+(A3*K3/E3)^2+(C3*Q3/E3)^2)</f>
+      <c r="AC3">
+        <f t="shared" ref="AC3:AC6" si="18">SQRT(((J3/E3-(A3*J3+C3*P3)/E3^2)*B3)^2+((P3/E3-(A3*J3+C3*P3)/E3^2)*D3)^2+(A3*K3/E3)^2+(C3*Q3/E3)^2)</f>
         <v>7.2408096213654502E-2</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:W6" si="13">S3-U3</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD6" si="19">Z3-AB3</f>
         <v>0.29164515271211289</v>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X6" si="14">SQRT(T3^2+V3^2)</f>
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE6" si="20">SQRT(AA3^2+AC3^2)</f>
         <v>0.1025050091437844</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:D6" si="15">A3</f>
+        <f t="shared" ref="A4:D6" si="21">A3</f>
         <v>206.137</v>
       </c>
       <c r="B4">
@@ -713,11 +797,11 @@
         <v>1E-3</v>
       </c>
       <c r="C4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>205.25800000000001</v>
       </c>
       <c r="D4">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1E-3</v>
       </c>
       <c r="E4">
@@ -770,32 +854,56 @@
       </c>
       <c r="S4">
         <f t="shared" si="10"/>
+        <v>91.562449999999998</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="11"/>
+        <v>0.14531022787470951</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="12"/>
+        <v>-87.568450000000013</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="13"/>
+        <v>0.14501556971925467</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="14"/>
+        <v>0.91466174489141883</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="15"/>
+        <v>4.1958995996136342E-3</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="16"/>
         <v>11.031392661310903</v>
       </c>
-      <c r="T4">
+      <c r="AA4">
         <f>SQRT(((G4/E4-(A4*G4+C4*M4)/E4^2)*B4)^2+((M4/E4-(A4*G4+C4*M4)/E4^2)*D4)^2+(A4*H4/E4)^2+(C4*N4/E4)^2)</f>
         <v>7.2659154515144375E-2</v>
       </c>
-      <c r="U4">
-        <f t="shared" si="11"/>
+      <c r="AB4">
+        <f t="shared" si="17"/>
         <v>11.239424194144318</v>
       </c>
-      <c r="V4">
-        <f t="shared" si="12"/>
+      <c r="AC4">
+        <f t="shared" si="18"/>
         <v>7.250442681641063E-2</v>
       </c>
-      <c r="W4">
-        <f t="shared" si="13"/>
+      <c r="AD4">
+        <f t="shared" si="19"/>
         <v>-0.2080315328334148</v>
       </c>
-      <c r="X4">
-        <f t="shared" si="14"/>
+      <c r="AE4">
+        <f t="shared" si="20"/>
         <v>0.10264621104956516</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>206.137</v>
       </c>
       <c r="B5">
@@ -803,11 +911,11 @@
         <v>1E-3</v>
       </c>
       <c r="C5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>205.25800000000001</v>
       </c>
       <c r="D5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1E-3</v>
       </c>
       <c r="E5">
@@ -860,32 +968,56 @@
       </c>
       <c r="S5">
         <f t="shared" si="10"/>
+        <v>133.79900000000001</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="11"/>
+        <v>0.14918713194508434</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="12"/>
+        <v>-125.71115</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="13"/>
+        <v>0.14829793989465939</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="14"/>
+        <v>0.88275840944531059</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="15"/>
+        <v>2.8658379519136967E-3</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="16"/>
         <v>-2.7527103422501535</v>
       </c>
-      <c r="T5">
+      <c r="AA5">
         <f>SQRT(((G5/E5-(A5*G5+C5*M5)/E5^2)*B5)^2+((M5/E5-(A5*G5+C5*M5)/E5^2)*D5)^2+(A5*H5/E5)^2+(C5*N5/E5)^2)</f>
         <v>7.4592694369911533E-2</v>
       </c>
-      <c r="U5">
-        <f t="shared" si="11"/>
+      <c r="AB5">
+        <f t="shared" si="17"/>
         <v>-2.8801742754530313</v>
       </c>
-      <c r="V5">
-        <f t="shared" si="12"/>
+      <c r="AC5">
+        <f t="shared" si="18"/>
         <v>7.4150705568643893E-2</v>
       </c>
-      <c r="W5">
-        <f t="shared" si="13"/>
+      <c r="AD5">
+        <f t="shared" si="19"/>
         <v>0.12746393320287774</v>
       </c>
-      <c r="X5">
-        <f t="shared" si="14"/>
+      <c r="AE5">
+        <f t="shared" si="20"/>
         <v>0.10517793109626537</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>206.137</v>
       </c>
       <c r="B6">
@@ -893,11 +1025,11 @@
         <v>1E-3</v>
       </c>
       <c r="C6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>205.25800000000001</v>
       </c>
       <c r="D6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>1E-3</v>
       </c>
       <c r="E6">
@@ -950,26 +1082,50 @@
       </c>
       <c r="S6">
         <f t="shared" si="10"/>
+        <v>88.267400000000009</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="11"/>
+        <v>0.14486047318022954</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="12"/>
+        <v>-84.473100000000017</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="13"/>
+        <v>0.14457984065560456</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="14"/>
+        <v>0.91587498208472418</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="15"/>
+        <v>4.3435225586824196E-3</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="16"/>
         <v>2.9899475055603504</v>
       </c>
-      <c r="T6">
+      <c r="AA6">
         <f>SQRT(((G6/E6-(A6*G6+C6*M6)/E6^2)*B6)^2+((M6/E6-(A6*G6+C6*M6)/E6^2)*D6)^2+(A6*H6/E6)^2+(C6*N6/E6)^2)</f>
         <v>7.24315095054959E-2</v>
       </c>
-      <c r="U6">
-        <f t="shared" si="11"/>
+      <c r="AB6">
+        <f t="shared" si="17"/>
         <v>3.2048060071221101</v>
       </c>
-      <c r="V6">
-        <f t="shared" si="12"/>
+      <c r="AC6">
+        <f t="shared" si="18"/>
         <v>7.2289195982637874E-2</v>
       </c>
-      <c r="W6">
-        <f t="shared" si="13"/>
+      <c r="AD6">
+        <f t="shared" si="19"/>
         <v>-0.21485850156175967</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="14"/>
+      <c r="AE6">
+        <f t="shared" si="20"/>
         <v>0.10233304170726565</v>
       </c>
     </row>
@@ -980,15 +1136,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29FA719-9B06-48B5-8E88-8E620C2DAB58}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1041,25 +1197,43 @@
         <v>11</v>
       </c>
       <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AC1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AD1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>406.87200000000001</v>
       </c>
@@ -1121,31 +1295,55 @@
         <v>0.10216840272804503</v>
       </c>
       <c r="S2">
+        <f>G2-M2</f>
+        <v>69.096199999999996</v>
+      </c>
+      <c r="T2">
+        <f>SQRT(H2^2+N2^2)</f>
+        <v>0.14381123116780553</v>
+      </c>
+      <c r="U2">
+        <f>J2-P2</f>
+        <v>-65.301900000000003</v>
+      </c>
+      <c r="V2">
+        <f>SQRT(K2^2+Q2^2)</f>
+        <v>0.14345077127711792</v>
+      </c>
+      <c r="W2">
+        <f>U2^2/S2^2</f>
+        <v>0.89318888035016231</v>
+      </c>
+      <c r="X2">
+        <f>2*ABS(U2/S2)*SQRT((V2/S2)^2+(U2*T2/S2^2)^2)</f>
+        <v>5.4058282091422683E-3</v>
+      </c>
+      <c r="Z2">
         <f>(G2*A2+M2*C2)/(A2+C2)</f>
         <v>-1.302026187411172</v>
       </c>
-      <c r="T2">
+      <c r="AA2">
         <f>SQRT(((G2/E2-(A2*G2+C2*M2)/E2^2)*B2)^2+((M2/E2-(A2*G2+C2*M2)/E2^2)*D2)^2+(A2*H2/E2)^2+(C2*N2/E2)^2)</f>
         <v>7.5224313409132049E-2</v>
       </c>
-      <c r="U2">
+      <c r="AB2">
         <f>(J2*A2+P2*C2)/(A2+C2)</f>
         <v>-1.6677196147877125</v>
       </c>
-      <c r="V2">
+      <c r="AC2">
         <f>SQRT(((J2/E2-(A2*J2+C2*P2)/E2^2)*B2)^2+((P2/E2-(A2*J2+C2*P2)/E2^2)*D2)^2+(A2*K2/E2)^2+(C2*Q2/E2)^2)</f>
         <v>7.5189397310317457E-2</v>
       </c>
-      <c r="W2">
-        <f>S2-U2</f>
+      <c r="AD2">
+        <f>Z2-AB2</f>
         <v>0.36569342737654043</v>
       </c>
-      <c r="X2">
-        <f>SQRT(T2^2+V2^2)</f>
+      <c r="AE2">
+        <f>SQRT(AA2^2+AC2^2)</f>
         <v>0.1063585576987771</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2</f>
         <v>406.87200000000001</v>
@@ -1211,33 +1409,57 @@
         <v>0.10748951958679508</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S6" si="10">(G3*A3+M3*C3)/(A3+C3)</f>
+        <f t="shared" ref="S3:S6" si="10">G3-M3</f>
+        <v>101.44760000000001</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T6" si="11">SQRT(H3^2+N3^2)</f>
+        <v>0.14593552716867819</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U6" si="12">J3-P3</f>
+        <v>-96.355250000000012</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V6" si="13">SQRT(K3^2+Q3^2)</f>
+        <v>0.14708328245249358</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W6" si="14">U3^2/S3^2</f>
+        <v>0.90212602300204614</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X6" si="15">2*ABS(U3/S3)*SQRT((V3/S3)^2+(U3*T3/S3^2)^2)</f>
+        <v>3.7844068164379369E-3</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z6" si="16">(G3*A3+M3*C3)/(A3+C3)</f>
         <v>14.609778025419443</v>
       </c>
-      <c r="T3">
+      <c r="AA3">
         <f>SQRT(((G3/E3-(A3*G3+C3*M3)/E3^2)*B3)^2+((M3/E3-(A3*G3+C3*M3)/E3^2)*D3)^2+(A3*H3/E3)^2+(C3*N3/E3)^2)</f>
         <v>7.6709028894345985E-2</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U6" si="11">(J3*A3+P3*C3)/(A3+C3)</f>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB6" si="17">(J3*A3+P3*C3)/(A3+C3)</f>
         <v>14.536317082155753</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V6" si="12">SQRT(((J3/E3-(A3*J3+C3*P3)/E3^2)*B3)^2+((P3/E3-(A3*J3+C3*P3)/E3^2)*D3)^2+(A3*K3/E3)^2+(C3*Q3/E3)^2)</f>
+      <c r="AC3">
+        <f t="shared" ref="AC3:AC6" si="18">SQRT(((J3/E3-(A3*J3+C3*P3)/E3^2)*B3)^2+((P3/E3-(A3*J3+C3*P3)/E3^2)*D3)^2+(A3*K3/E3)^2+(C3*Q3/E3)^2)</f>
         <v>7.5843780596030946E-2</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:W6" si="13">S3-U3</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD6" si="19">Z3-AB3</f>
         <v>7.3460943263690126E-2</v>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X6" si="14">SQRT(T3^2+V3^2)</f>
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE6" si="20">SQRT(AA3^2+AC3^2)</f>
         <v>0.10787286113296748</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A6" si="15">A3</f>
+        <f t="shared" ref="A4:A6" si="21">A3</f>
         <v>406.87200000000001</v>
       </c>
       <c r="B4">
@@ -1302,32 +1524,56 @@
       </c>
       <c r="S4">
         <f t="shared" si="10"/>
+        <v>91.262900000000002</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="11"/>
+        <v>0.14507932071801274</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="12"/>
+        <v>-87.069200000000009</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="13"/>
+        <v>0.14623505739049034</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="14"/>
+        <v>0.910207853520965</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="15"/>
+        <v>4.2098115025505185E-3</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="16"/>
         <v>15.129237810269059</v>
       </c>
-      <c r="T4">
+      <c r="AA4">
         <f>SQRT(((G4/E4-(A4*G4+C4*M4)/E4^2)*B4)^2+((M4/E4-(A4*G4+C4*M4)/E4^2)*D4)^2+(A4*H4/E4)^2+(C4*N4/E4)^2)</f>
         <v>7.6378053992139344E-2</v>
       </c>
-      <c r="U4">
-        <f t="shared" si="11"/>
+      <c r="AB4">
+        <f t="shared" si="17"/>
         <v>14.917290513616392</v>
       </c>
-      <c r="V4">
-        <f t="shared" si="12"/>
+      <c r="AC4">
+        <f t="shared" si="18"/>
         <v>7.559772297740637E-2</v>
       </c>
-      <c r="W4">
-        <f t="shared" si="13"/>
+      <c r="AD4">
+        <f t="shared" si="19"/>
         <v>0.21194729665266721</v>
       </c>
-      <c r="X4">
-        <f t="shared" si="14"/>
+      <c r="AE4">
+        <f t="shared" si="20"/>
         <v>0.10746451903300376</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>406.87200000000001</v>
       </c>
       <c r="B5">
@@ -1392,32 +1638,56 @@
       </c>
       <c r="S5">
         <f t="shared" si="10"/>
+        <v>75.786149999999992</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="11"/>
+        <v>0.14397962197825082</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="12"/>
+        <v>-71.193049999999999</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="13"/>
+        <v>0.14436582352135841</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="14"/>
+        <v>0.88246097337006446</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="15"/>
+        <v>4.9042285534956461E-3</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="16"/>
         <v>8.6364154245013331</v>
       </c>
-      <c r="T5">
+      <c r="AA5">
         <f>SQRT(((G5/E5-(A5*G5+C5*M5)/E5^2)*B5)^2+((M5/E5-(A5*G5+C5*M5)/E5^2)*D5)^2+(A5*H5/E5)^2+(C5*N5/E5)^2)</f>
         <v>7.5634692818180735E-2</v>
       </c>
-      <c r="U5">
-        <f t="shared" si="11"/>
+      <c r="AB5">
+        <f t="shared" si="17"/>
         <v>8.3955370254684443</v>
       </c>
-      <c r="V5">
-        <f t="shared" si="12"/>
+      <c r="AC5">
+        <f t="shared" si="18"/>
         <v>7.521228543362421E-2</v>
       </c>
-      <c r="W5">
-        <f t="shared" si="13"/>
+      <c r="AD5">
+        <f t="shared" si="19"/>
         <v>0.24087839903288888</v>
       </c>
-      <c r="X5">
-        <f t="shared" si="14"/>
+      <c r="AE5">
+        <f t="shared" si="20"/>
         <v>0.10666533943999579</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>406.87200000000001</v>
       </c>
       <c r="B6">
@@ -1482,26 +1752,50 @@
       </c>
       <c r="S6">
         <f t="shared" si="10"/>
+        <v>107.43859999999999</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="11"/>
+        <v>0.14647333269916407</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="12"/>
+        <v>-100.74865</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="13"/>
+        <v>0.14804902693702518</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="14"/>
+        <v>0.87934194524674902</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="15"/>
+        <v>3.5252917224205351E-3</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="16"/>
         <v>19.690239916684366</v>
       </c>
-      <c r="T6">
+      <c r="AA6">
         <f>SQRT(((G6/E6-(A6*G6+C6*M6)/E6^2)*B6)^2+((M6/E6-(A6*G6+C6*M6)/E6^2)*D6)^2+(A6*H6/E6)^2+(C6*N6/E6)^2)</f>
         <v>7.7222232780007685E-2</v>
       </c>
-      <c r="U6">
-        <f t="shared" si="11"/>
+      <c r="AB6">
+        <f t="shared" si="17"/>
         <v>19.104851695228138</v>
       </c>
-      <c r="V6">
-        <f t="shared" si="12"/>
+      <c r="AC6">
+        <f t="shared" si="18"/>
         <v>7.6000019131542654E-2</v>
       </c>
-      <c r="W6">
-        <f t="shared" si="13"/>
+      <c r="AD6">
+        <f t="shared" si="19"/>
         <v>0.5853882214562276</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="14"/>
+      <c r="AE6">
+        <f t="shared" si="20"/>
         <v>0.10834794019050174</v>
       </c>
     </row>
@@ -1512,15 +1806,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F65CE6B8-7EAA-4E76-AF4E-B2C1B6276440}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:X6"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1573,25 +1867,43 @@
         <v>11</v>
       </c>
       <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AC1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AD1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>206.161</v>
       </c>
@@ -1654,31 +1966,55 @@
         <v>0.10028563062074247</v>
       </c>
       <c r="S2">
+        <f>G2-M2</f>
+        <v>110.73365000000001</v>
+      </c>
+      <c r="T2">
+        <f>SQRT(H2^2+N2^2)</f>
+        <v>0.14718242635926343</v>
+      </c>
+      <c r="U2">
+        <f>J2-P2</f>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f>SQRT(K2^2+Q2^2)</f>
+        <v>0.14182529893499254</v>
+      </c>
+      <c r="W2">
+        <f>U2^2/S2^2</f>
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <f>2*ABS(U2/S2)*SQRT((V2/S2)^2+(U2*T2/S2^2)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2">
         <f>(G2*A2+M2*C2)/(A2+C2)</f>
         <v>-15.341290634731328</v>
       </c>
-      <c r="T2">
+      <c r="AA2">
         <f>SQRT(((G2/E2-(A2*G2+C2*M2)/E2^2)*B2)^2+((M2/E2-(A2*G2+C2*M2)/E2^2)*D2)^2+(A2*H2/E2)^2+(C2*N2/E2)^2)</f>
         <v>7.3587034378384347E-2</v>
       </c>
-      <c r="U2">
+      <c r="AB2">
         <f>(J2*A2+P2*C2)/(A2+C2)</f>
         <v>-15.077349999999999</v>
       </c>
-      <c r="V2">
+      <c r="AC2">
         <f>SQRT(((J2/E2-(A2*J2+C2*P2)/E2^2)*B2)^2+((P2/E2-(A2*J2+C2*P2)/E2^2)*D2)^2+(A2*K2/E2)^2+(C2*Q2/E2)^2)</f>
         <v>7.0912734087977658E-2</v>
       </c>
-      <c r="W2">
-        <f>S2-U2</f>
+      <c r="AD2">
+        <f>Z2-AB2</f>
         <v>-0.26394063473132867</v>
       </c>
-      <c r="X2">
-        <f>SQRT(T2^2+V2^2)</f>
+      <c r="AE2">
+        <f>SQRT(AA2^2+AC2^2)</f>
         <v>0.10219426346149645</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2</f>
         <v>206.161</v>
@@ -1745,45 +2081,69 @@
         <v>0.10011315460517664</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S6" si="11">(G3*A3+M3*C3)/(A3+C3)</f>
+        <f t="shared" ref="S3:S6" si="11">G3-M3</f>
+        <v>123.2149</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T6" si="12">SQRT(H3^2+N3^2)</f>
+        <v>0.14818067270734062</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U6" si="13">J3-P3</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V6" si="14">SQRT(K3^2+Q3^2)</f>
+        <v>0.14158138101459528</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W6" si="15">U3^2/S3^2</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X6" si="16">2*ABS(U3/S3)*SQRT((V3/S3)^2+(U3*T3/S3^2)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z6" si="17">(G3*A3+M3*C3)/(A3+C3)</f>
         <v>-9.5902747008642493</v>
       </c>
-      <c r="T3">
+      <c r="AA3">
         <f>SQRT(((G3/E3-(A3*G3+C3*M3)/E3^2)*B3)^2+((M3/E3-(A3*G3+C3*M3)/E3^2)*D3)^2+(A3*H3/E3)^2+(C3*N3/E3)^2)</f>
         <v>7.4087595942222015E-2</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U6" si="12">(J3*A3+P3*C3)/(A3+C3)</f>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB6" si="18">(J3*A3+P3*C3)/(A3+C3)</f>
         <v>-9.4857500000000012</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V6" si="13">SQRT(((J3/E3-(A3*J3+C3*P3)/E3^2)*B3)^2+((P3/E3-(A3*J3+C3*P3)/E3^2)*D3)^2+(A3*K3/E3)^2+(C3*Q3/E3)^2)</f>
+      <c r="AC3">
+        <f t="shared" ref="AC3:AC6" si="19">SQRT(((J3/E3-(A3*J3+C3*P3)/E3^2)*B3)^2+((P3/E3-(A3*J3+C3*P3)/E3^2)*D3)^2+(A3*K3/E3)^2+(C3*Q3/E3)^2)</f>
         <v>7.0790774982244689E-2</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:W6" si="14">S3-U3</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD6" si="20">Z3-AB3</f>
         <v>-0.10452470086424803</v>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X6" si="15">SQRT(T3^2+V3^2)</f>
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE6" si="21">SQRT(AA3^2+AC3^2)</f>
         <v>0.10247099928801685</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:D6" si="16">A3</f>
+        <f t="shared" ref="A4:D6" si="22">A3</f>
         <v>206.161</v>
       </c>
       <c r="B4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1E-3</v>
       </c>
       <c r="C4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>205.52500000000001</v>
       </c>
       <c r="D4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1E-3</v>
       </c>
       <c r="E4">
@@ -1837,44 +2197,68 @@
       </c>
       <c r="S4">
         <f t="shared" si="11"/>
+        <v>118.92134999999999</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="12"/>
+        <v>0.14824040534550628</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="14"/>
+        <v>0.1420874992671769</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="17"/>
         <v>19.812233817885474</v>
       </c>
-      <c r="T4">
+      <c r="AA4">
         <f>SQRT(((G4/E4-(A4*G4+C4*M4)/E4^2)*B4)^2+((M4/E4-(A4*G4+C4*M4)/E4^2)*D4)^2+(A4*H4/E4)^2+(C4*N4/E4)^2)</f>
         <v>7.4126722686335453E-2</v>
       </c>
-      <c r="U4">
-        <f t="shared" si="12"/>
+      <c r="AB4">
+        <f t="shared" si="18"/>
         <v>19.370899999999999</v>
       </c>
-      <c r="V4">
-        <f t="shared" si="13"/>
+      <c r="AC4">
+        <f t="shared" si="19"/>
         <v>7.1043834410512444E-2</v>
       </c>
-      <c r="W4">
-        <f t="shared" si="14"/>
+      <c r="AD4">
+        <f t="shared" si="20"/>
         <v>0.4413338178854751</v>
       </c>
-      <c r="X4">
-        <f t="shared" si="15"/>
+      <c r="AE4">
+        <f t="shared" si="21"/>
         <v>0.10267422960005684</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>206.161</v>
       </c>
       <c r="B5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1E-3</v>
       </c>
       <c r="C5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>205.52500000000001</v>
       </c>
       <c r="D5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1E-3</v>
       </c>
       <c r="E5">
@@ -1928,44 +2312,68 @@
       </c>
       <c r="S5">
         <f t="shared" si="11"/>
+        <v>133.19990000000001</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="12"/>
+        <v>0.14913518952279506</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="14"/>
+        <v>0.14144833819455074</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="17"/>
         <v>4.2965880462294139</v>
       </c>
-      <c r="T5">
+      <c r="AA5">
         <f>SQRT(((G5/E5-(A5*G5+C5*M5)/E5^2)*B5)^2+((M5/E5-(A5*G5+C5*M5)/E5^2)*D5)^2+(A5*H5/E5)^2+(C5*N5/E5)^2)</f>
         <v>7.4569490871861918E-2</v>
       </c>
-      <c r="U5">
-        <f t="shared" si="12"/>
+      <c r="AB5">
+        <f t="shared" si="18"/>
         <v>3.8941499999999998</v>
       </c>
-      <c r="V5">
-        <f t="shared" si="13"/>
+      <c r="AC5">
+        <f t="shared" si="19"/>
         <v>7.0724253492842018E-2</v>
       </c>
-      <c r="W5">
-        <f t="shared" si="14"/>
+      <c r="AD5">
+        <f t="shared" si="20"/>
         <v>0.40243804622941415</v>
       </c>
-      <c r="X5">
-        <f t="shared" si="15"/>
+      <c r="AE5">
+        <f t="shared" si="21"/>
         <v>0.10277416504651583</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>206.161</v>
       </c>
       <c r="B6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1E-3</v>
       </c>
       <c r="C6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>205.52500000000001</v>
       </c>
       <c r="D6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="22"/>
         <v>1E-3</v>
       </c>
       <c r="E6">
@@ -2019,26 +2427,50 @@
       </c>
       <c r="S6">
         <f t="shared" si="11"/>
+        <v>165.65115000000003</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="12"/>
+        <v>0.15319151813661228</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="14"/>
+        <v>0.14146570255719229</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="17"/>
         <v>5.5697794742837976</v>
       </c>
-      <c r="T6">
+      <c r="AA6">
         <f>SQRT(((G6/E6-(A6*G6+C6*M6)/E6^2)*B6)^2+((M6/E6-(A6*G6+C6*M6)/E6^2)*D6)^2+(A6*H6/E6)^2+(C6*N6/E6)^2)</f>
         <v>7.6598666556204134E-2</v>
       </c>
-      <c r="U6">
-        <f t="shared" si="12"/>
+      <c r="AB6">
+        <f t="shared" si="18"/>
         <v>4.9924999999999997</v>
       </c>
-      <c r="V6">
-        <f t="shared" si="13"/>
+      <c r="AC6">
+        <f t="shared" si="19"/>
         <v>7.0732935684523296E-2</v>
       </c>
-      <c r="W6">
-        <f t="shared" si="14"/>
+      <c r="AD6">
+        <f t="shared" si="20"/>
         <v>0.57727947428379789</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="15"/>
+      <c r="AE6">
+        <f t="shared" si="21"/>
         <v>0.10426170873690617</v>
       </c>
     </row>
@@ -2049,15 +2481,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A716F036-AE53-4E0C-BF10-0BF014F704B3}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2110,25 +2542,43 @@
         <v>11</v>
       </c>
       <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AC1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AD1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>406.89600000000002</v>
       </c>
@@ -2191,31 +2641,55 @@
         <v>0.10004365961419046</v>
       </c>
       <c r="S2">
+        <f>G2-M2</f>
+        <v>68.29740000000001</v>
+      </c>
+      <c r="T2">
+        <f>SQRT(H2^2+N2^2)</f>
+        <v>0.14352006868030687</v>
+      </c>
+      <c r="U2">
+        <f>J2-P2</f>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f>SQRT(K2^2+Q2^2)</f>
+        <v>0.14148310025582564</v>
+      </c>
+      <c r="W2">
+        <f>U2^2/S2^2</f>
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <f>2*ABS(U2/S2)*SQRT((V2/S2)^2+(U2*T2/S2^2)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2">
         <f>(G2*A2+M2*C2)/(A2+C2)</f>
         <v>6.5355314983483579</v>
       </c>
-      <c r="T2">
+      <c r="AA2">
         <f>SQRT(((G2/E2-(A2*G2+C2*M2)/E2^2)*B2)^2+((M2/E2-(A2*G2+C2*M2)/E2^2)*D2)^2+(A2*H2/E2)^2+(C2*N2/E2)^2)</f>
         <v>7.5364058983625304E-2</v>
       </c>
-      <c r="U2">
+      <c r="AB2">
         <f>(J2*A2+P2*C2)/(A2+C2)</f>
         <v>5.8911499999999997</v>
       </c>
-      <c r="V2">
+      <c r="AC2">
         <f>SQRT(((J2/E2-(A2*J2+C2*P2)/E2^2)*B2)^2+((P2/E2-(A2*J2+C2*P2)/E2^2)*D2)^2+(A2*K2/E2)^2+(C2*Q2/E2)^2)</f>
         <v>7.4467601689459706E-2</v>
       </c>
-      <c r="W2">
-        <f>S2-U2</f>
+      <c r="AD2">
+        <f>Z2-AB2</f>
         <v>0.64438149834835823</v>
       </c>
-      <c r="X2">
-        <f>SQRT(T2^2+V2^2)</f>
+      <c r="AE2">
+        <f>SQRT(AA2^2+AC2^2)</f>
         <v>0.10594887959703668</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2</f>
         <v>406.89600000000002</v>
@@ -2282,45 +2756,69 @@
         <v>0.1004710342536594</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S6" si="11">(G3*A3+M3*C3)/(A3+C3)</f>
+        <f t="shared" ref="S3:S6" si="11">G3-M3</f>
+        <v>83.175049999999999</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T6" si="12">SQRT(H3^2+N3^2)</f>
+        <v>0.14453187565724041</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U6" si="13">J3-P3</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V6" si="14">SQRT(K3^2+Q3^2)</f>
+        <v>0.1420874992671769</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W6" si="15">U3^2/S3^2</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X6" si="16">2*ABS(U3/S3)*SQRT((V3/S3)^2+(U3*T3/S3^2)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f>(G3*A3+M3*C3)/(A3+C3)</f>
         <v>19.815226883222486</v>
       </c>
-      <c r="T3">
+      <c r="AA3">
         <f>SQRT(((G3/E3-(A3*G3+C3*M3)/E3^2)*B3)^2+((M3/E3-(A3*G3+C3*M3)/E3^2)*D3)^2+(A3*H3/E3)^2+(C3*N3/E3)^2)</f>
         <v>7.6349680234528192E-2</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U6" si="12">(J3*A3+P3*C3)/(A3+C3)</f>
+      <c r="AB3">
+        <f>(J3*A3+P3*C3)/(A3+C3)</f>
         <v>19.370899999999995</v>
       </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V6" si="13">SQRT(((J3/E3-(A3*J3+C3*P3)/E3^2)*B3)^2+((P3/E3-(A3*J3+C3*P3)/E3^2)*D3)^2+(A3*K3/E3)^2+(C3*Q3/E3)^2)</f>
+      <c r="AC3">
+        <f>SQRT(((J3/E3-(A3*J3+C3*P3)/E3^2)*B3)^2+((P3/E3-(A3*J3+C3*P3)/E3^2)*D3)^2+(A3*K3/E3)^2+(C3*Q3/E3)^2)</f>
         <v>7.4785718445152999E-2</v>
       </c>
-      <c r="W3">
-        <f t="shared" ref="W3:W6" si="14">S3-U3</f>
+      <c r="AD3">
+        <f t="shared" ref="AD3:AD6" si="17">Z3-AB3</f>
         <v>0.44432688322249092</v>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X6" si="15">SQRT(T3^2+V3^2)</f>
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE6" si="18">SQRT(AA3^2+AC3^2)</f>
         <v>0.10687458704141224</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:D6" si="16">A3</f>
+        <f t="shared" ref="A4:D6" si="19">A3</f>
         <v>406.89600000000002</v>
       </c>
       <c r="B4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
       <c r="C4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>205.52500000000001</v>
       </c>
       <c r="D4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1.4E-3</v>
       </c>
       <c r="E4">
@@ -2374,44 +2872,68 @@
       </c>
       <c r="S4">
         <f t="shared" si="11"/>
+        <v>139.9897</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="12"/>
+        <v>0.15109254685787782</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="14"/>
+        <v>0.14145569924184748</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <f>(G4*A4+M4*C4)/(A4+C4)</f>
         <v>-3.8445461101105307</v>
       </c>
-      <c r="T4">
+      <c r="AA4">
         <f>SQRT(((G4/E4-(A4*G4+C4*M4)/E4^2)*B4)^2+((M4/E4-(A4*G4+C4*M4)/E4^2)*D4)^2+(A4*H4/E4)^2+(C4*N4/E4)^2)</f>
         <v>7.7544861124720421E-2</v>
       </c>
-      <c r="U4">
-        <f t="shared" si="12"/>
+      <c r="AB4">
+        <f>(J4*A4+P4*C4)/(A4+C4)</f>
         <v>-4.3934000000000006</v>
       </c>
-      <c r="V4">
-        <f t="shared" si="13"/>
+      <c r="AC4">
+        <f>SQRT(((J4/E4-(A4*J4+C4*P4)/E4^2)*B4)^2+((P4/E4-(A4*J4+C4*P4)/E4^2)*D4)^2+(A4*K4/E4)^2+(C4*Q4/E4)^2)</f>
         <v>7.4453179558540014E-2</v>
       </c>
-      <c r="W4">
-        <f t="shared" si="14"/>
+      <c r="AD4">
+        <f t="shared" si="17"/>
         <v>0.54885388988946993</v>
       </c>
-      <c r="X4">
-        <f t="shared" si="15"/>
+      <c r="AE4">
+        <f t="shared" si="18"/>
         <v>0.10750107642823106</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>406.89600000000002</v>
       </c>
       <c r="B5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
       <c r="C5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>205.52500000000001</v>
       </c>
       <c r="D5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1.4E-3</v>
       </c>
       <c r="E5">
@@ -2465,44 +2987,68 @@
       </c>
       <c r="S5">
         <f t="shared" si="11"/>
+        <v>139.9897</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="12"/>
+        <v>0.15220955287366167</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="14"/>
+        <v>0.14174911967275142</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <f>(G5*A5+M5*C5)/(A5+C5)</f>
         <v>-14.328796110110529</v>
       </c>
-      <c r="T5">
+      <c r="AA5">
         <f>SQRT(((G5/E5-(A5*G5+C5*M5)/E5^2)*B5)^2+((M5/E5-(A5*G5+C5*M5)/E5^2)*D5)^2+(A5*H5/E5)^2+(C5*N5/E5)^2)</f>
         <v>7.736674896077024E-2</v>
       </c>
-      <c r="U5">
-        <f t="shared" si="12"/>
+      <c r="AB5">
+        <f>(J5*A5+P5*C5)/(A5+C5)</f>
         <v>-13.579599999999999</v>
       </c>
-      <c r="V5">
-        <f t="shared" si="13"/>
+      <c r="AC5">
+        <f>SQRT(((J5/E5-(A5*J5+C5*P5)/E5^2)*B5)^2+((P5/E5-(A5*J5+C5*P5)/E5^2)*D5)^2+(A5*K5/E5)^2+(C5*Q5/E5)^2)</f>
         <v>7.4607617196226758E-2</v>
       </c>
-      <c r="W5">
-        <f t="shared" si="14"/>
+      <c r="AD5">
+        <f t="shared" si="17"/>
         <v>-0.74919611011053</v>
       </c>
-      <c r="X5">
-        <f t="shared" si="15"/>
+      <c r="AE5">
+        <f t="shared" si="18"/>
         <v>0.10747981386501167</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>406.89600000000002</v>
       </c>
       <c r="B6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
       <c r="C6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>205.52500000000001</v>
       </c>
       <c r="D6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>1.4E-3</v>
       </c>
       <c r="E6">
@@ -2556,26 +3102,50 @@
       </c>
       <c r="S6">
         <f t="shared" si="11"/>
+        <v>130.90335000000002</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="12"/>
+        <v>0.14887435449062408</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="14"/>
+        <v>0.14217952131724176</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <f>(G6*A6+M6*C6)/(A6+C6)</f>
         <v>25.365481205167686</v>
       </c>
-      <c r="T6">
+      <c r="AA6">
         <f>SQRT(((G6/E6-(A6*G6+C6*M6)/E6^2)*B6)^2+((M6/E6-(A6*G6+C6*M6)/E6^2)*D6)^2+(A6*H6/E6)^2+(C6*N6/E6)^2)</f>
         <v>7.8623421641670035E-2</v>
       </c>
-      <c r="U6">
-        <f t="shared" si="12"/>
+      <c r="AB6">
+        <f>(J6*A6+P6*C6)/(A6+C6)</f>
         <v>20.668949999999999</v>
       </c>
-      <c r="V6">
-        <f t="shared" si="13"/>
+      <c r="AC6">
+        <f>SQRT(((J6/E6-(A6*J6+C6*P6)/E6^2)*B6)^2+((P6/E6-(A6*J6+C6*P6)/E6^2)*D6)^2+(A6*K6/E6)^2+(C6*Q6/E6)^2)</f>
         <v>7.4834152932088088E-2</v>
       </c>
-      <c r="W6">
-        <f t="shared" si="14"/>
+      <c r="AD6">
+        <f t="shared" si="17"/>
         <v>4.6965312051676875</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="15"/>
+      <c r="AE6">
+        <f t="shared" si="18"/>
         <v>0.10854396747727152</v>
       </c>
     </row>

</xml_diff>